<commit_message>
2016.07.18 - Additional work on databuild
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Source File</t>
   </si>
@@ -144,6 +144,111 @@
   </si>
   <si>
     <t>Percent of Residents Mode of Transportation to Work - Walked to Work,  Population Aged 16 Years and Older</t>
+  </si>
+  <si>
+    <t>Food_afford_cdp_co_region_ca4-14-13.xls</t>
+  </si>
+  <si>
+    <t>Food Affordability</t>
+  </si>
+  <si>
+    <t>affordability_ratio</t>
+  </si>
+  <si>
+    <t>ave_fam_size</t>
+  </si>
+  <si>
+    <t>median_income</t>
+  </si>
+  <si>
+    <t>Median income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average family size for a female headed family w/children &lt;18 yrs, specific to a geography, all races combined </t>
+  </si>
+  <si>
+    <t>Ratio of food cost to income,  female headed family w/children &lt;18 yrs</t>
+  </si>
+  <si>
+    <t>Access to Healthy Foods</t>
+  </si>
+  <si>
+    <t>HCI_RetailFoodEnvironment_75_CA_CO_RE_PL_CT_11-15-13.xls</t>
+  </si>
+  <si>
+    <t>hfood_acc</t>
+  </si>
+  <si>
+    <t>Modified retail food environment index: percentage of healthy food retailers</t>
+  </si>
+  <si>
+    <t>HCI_MilesByOccurrence_39_CA_CO_PL_RE_10-3-13.xls</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>Miles per capita by car, pub transit, &amp; walk/bike</t>
+  </si>
+  <si>
+    <t>Percent of residents by time walking &amp; biking</t>
+  </si>
+  <si>
+    <t>HCI_Walk_Bicycle_778_PL_CO_RE_CA-3-26-14.xlsx</t>
+  </si>
+  <si>
+    <t>HCI_CHAS_IncomeCrowding_PL_CO_RE_ST.xls</t>
+  </si>
+  <si>
+    <t>Percent of household overcrowding</t>
+  </si>
+  <si>
+    <t>HCI_JobHouseRatio_PL-MS-CO-768-4-24-15.xlsx</t>
+  </si>
+  <si>
+    <t>Jobs to Housing Ratio</t>
+  </si>
+  <si>
+    <t>job_house_low</t>
+  </si>
+  <si>
+    <t>job_house_tot</t>
+  </si>
+  <si>
+    <t>2007-2011</t>
+  </si>
+  <si>
+    <t>Jobs to housing ratio - Low wage jobs to affordable housing</t>
+  </si>
+  <si>
+    <t>Jobs to housing ratio - Total jobs to total housing</t>
+  </si>
+  <si>
+    <t>HCI_JobsMatch_PL-MS-CO_769_4-24-15.xlsx</t>
+  </si>
+  <si>
+    <t>job_match</t>
+  </si>
+  <si>
+    <t>Jobs to employed residents ratio - All industry sectors</t>
+  </si>
+  <si>
+    <t>ozone_zcta_place_co_region_ca4-14-13.xls</t>
+  </si>
+  <si>
+    <t>Avg. No. Unhealthy Ozone Days</t>
+  </si>
+  <si>
+    <t>Jobs to Employed Residents Ratio</t>
+  </si>
+  <si>
+    <t>2007-2009</t>
+  </si>
+  <si>
+    <t>ozone</t>
+  </si>
+  <si>
+    <t>Mean number of unhrealthy days of ozone exposure</t>
   </si>
 </sst>
 </file>
@@ -169,6 +274,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -508,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,22 +659,22 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>2010</v>
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -576,22 +682,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>2010</v>
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -599,22 +705,22 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,91 +728,56 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>2009</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,22 +785,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -737,22 +808,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,61 +831,322 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>2011</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>2010</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>2010</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
         <v>31</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E24" t="s">
         <v>25</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F24" t="s">
         <v>32</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G24" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="http://www.cdph.ca.gov/programs/Pages/HealthyCommunityIndicators.aspx"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A10" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
-    <hyperlink ref="A12" r:id="rId10"/>
+    <hyperlink ref="A14" r:id="rId1"/>
+    <hyperlink ref="A15:A16" r:id="rId2" display="http://www.cdph.ca.gov/programs/Pages/HealthyCommunityIndicators.aspx"/>
+    <hyperlink ref="A17" r:id="rId3"/>
+    <hyperlink ref="A18" r:id="rId4"/>
+    <hyperlink ref="A19" r:id="rId5"/>
+    <hyperlink ref="A20" r:id="rId6"/>
+    <hyperlink ref="A21" r:id="rId7"/>
+    <hyperlink ref="A22" r:id="rId8"/>
+    <hyperlink ref="A23" r:id="rId9"/>
+    <hyperlink ref="A24" r:id="rId10"/>
+    <hyperlink ref="A2" r:id="rId11"/>
+    <hyperlink ref="A3" r:id="rId12"/>
+    <hyperlink ref="A4" r:id="rId13"/>
+    <hyperlink ref="A5" r:id="rId14"/>
+    <hyperlink ref="A9" r:id="rId15"/>
+    <hyperlink ref="A10" r:id="rId16"/>
+    <hyperlink ref="A11" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2016.08.18 - Download HCI poverty/unemployment files; databuild work.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data_science\CA_Housing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crsalviati/Desktop/data_science/CA_Housing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="94">
   <si>
     <t>Source File</t>
   </si>
@@ -249,6 +255,63 @@
   </si>
   <si>
     <t>Mean number of unhrealthy days of ozone exposure</t>
+  </si>
+  <si>
+    <t>PM25_zcta_place_co_region_ca4-14-13.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Ambient PM2.5 Concentration  </t>
+  </si>
+  <si>
+    <t>pm25_conc</t>
+  </si>
+  <si>
+    <t>Mean ambient PM2.5 concentration (micrograms/cu m.)</t>
+  </si>
+  <si>
+    <t>HCI_Smoking_755_06NOV15.xlsx</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Place Level Data?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Prevalence  of Smoking</t>
+  </si>
+  <si>
+    <t>ed_attain_ge_hs_output04-14-13.xlsx</t>
+  </si>
+  <si>
+    <t>HS or greater educational attainement</t>
+  </si>
+  <si>
+    <t>Percent of population aged 25 years old and over attaining at least a high school degree or GED equivalency</t>
+  </si>
+  <si>
+    <t>p_hs_edatt</t>
+  </si>
+  <si>
+    <t>livewage_s</t>
+  </si>
+  <si>
+    <t>livewage_m</t>
+  </si>
+  <si>
+    <t>HCI_Living_Wage_770_PL_CO_RE_CA_9-29-13.xls</t>
+  </si>
+  <si>
+    <t>Living Wage</t>
+  </si>
+  <si>
+    <t>Percent of families living below the living wage - Single mother, two children</t>
+  </si>
+  <si>
+    <t>Percent of families living below the living wage - Married couple, two children</t>
   </si>
 </sst>
 </file>
@@ -397,9 +460,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -432,9 +495,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -614,24 +677,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="150.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -639,22 +703,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -662,22 +729,25 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -685,22 +755,25 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -708,22 +781,25 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -731,56 +807,68 @@
         <v>49</v>
       </c>
       <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>2009</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>50</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>56</v>
       </c>
       <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -788,22 +876,25 @@
         <v>59</v>
       </c>
       <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>63</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -811,22 +902,25 @@
         <v>59</v>
       </c>
       <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -834,46 +928,54 @@
         <v>66</v>
       </c>
       <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>2011</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B12" t="s">
         <v>69</v>
       </c>
       <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>73</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -881,22 +983,25 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2010</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>7</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -904,22 +1009,25 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>2010</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -927,22 +1035,25 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -950,22 +1061,25 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>19</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -973,22 +1087,25 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>26</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -996,22 +1113,25 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1019,22 +1139,25 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>28</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1042,22 +1165,25 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
         <v>23</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>25</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>29</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1065,22 +1191,25 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>30</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1088,22 +1217,25 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>31</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1111,19 +1243,143 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>25</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>32</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28">
+        <v>2010</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29">
+        <v>2010</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1145,8 +1401,14 @@
     <hyperlink ref="A9" r:id="rId15"/>
     <hyperlink ref="A10" r:id="rId16"/>
     <hyperlink ref="A11" r:id="rId17"/>
+    <hyperlink ref="A12" r:id="rId18"/>
+    <hyperlink ref="A25" r:id="rId19"/>
+    <hyperlink ref="A26" r:id="rId20"/>
+    <hyperlink ref="A27" r:id="rId21"/>
+    <hyperlink ref="A28" r:id="rId22"/>
+    <hyperlink ref="A29" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2016.07.18 - Databuild work.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
   <si>
     <t>Source File</t>
   </si>
@@ -312,6 +312,51 @@
   </si>
   <si>
     <t>Percent of families living below the living wage - Married couple, two children</t>
+  </si>
+  <si>
+    <t>poverty_child</t>
+  </si>
+  <si>
+    <t>poverty_conc</t>
+  </si>
+  <si>
+    <t>poverty_all</t>
+  </si>
+  <si>
+    <t>HCI_PovertyRate_754_CT_PL_CO_RE_CA_1-22-14.xlsx</t>
+  </si>
+  <si>
+    <t>Poverty Rate</t>
+  </si>
+  <si>
+    <t>Poverty rate (percent) - Child &lt;18</t>
+  </si>
+  <si>
+    <t>Poverty rate (percent) - Concentrated</t>
+  </si>
+  <si>
+    <t>Poverty rate (percent) - Overall</t>
+  </si>
+  <si>
+    <t>2000; 2005-2007; 2008-2011</t>
+  </si>
+  <si>
+    <t>2000; 2005-2007; 2008-2012</t>
+  </si>
+  <si>
+    <t>unemp_rate</t>
+  </si>
+  <si>
+    <t>2004;2005;2006;2007;2008;2009;2010;2011;2012;2013</t>
+  </si>
+  <si>
+    <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>HCI_Unemployment_290_CA_RE_CO_CD_PL_CT-5-22-14.xlsx</t>
+  </si>
+  <si>
+    <t>Unemployment rate (percent)</t>
   </si>
 </sst>
 </file>
@@ -677,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1380,6 +1425,110 @@
       </c>
       <c r="H29" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1407,8 +1556,12 @@
     <hyperlink ref="A27" r:id="rId21"/>
     <hyperlink ref="A28" r:id="rId22"/>
     <hyperlink ref="A29" r:id="rId23"/>
+    <hyperlink ref="A30" r:id="rId24"/>
+    <hyperlink ref="A31" r:id="rId25"/>
+    <hyperlink ref="A32" r:id="rId26"/>
+    <hyperlink ref="A33" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId24"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2016.07.19 - Download additional HCI files; additional databuild work.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crsalviati/Desktop/data_science/CA_Housing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data_science\CA_Housing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="175">
   <si>
     <t>Source File</t>
   </si>
@@ -357,6 +354,204 @@
   </si>
   <si>
     <t>Unemployment rate (percent)</t>
+  </si>
+  <si>
+    <t>HCI_Licensed_Daycare_Centers_760_CA_RE_CO_CD_PL_CT_110215.xlsx</t>
+  </si>
+  <si>
+    <t>Daycare Centers</t>
+  </si>
+  <si>
+    <t>day_care</t>
+  </si>
+  <si>
+    <t>inf_care</t>
+  </si>
+  <si>
+    <t>Number of licensed infant center slots per 1,000 children population</t>
+  </si>
+  <si>
+    <t>Number of licensed day care center slots per 1,000 children population</t>
+  </si>
+  <si>
+    <t>2000;2001;2002;2003;2004;2005;2006;2007;2008;2009;2011;2012;2013</t>
+  </si>
+  <si>
+    <t>Violent Crime</t>
+  </si>
+  <si>
+    <t>HCI_Crime_752_PL_CO_RE_CA_2000-2013_21OCT15.xlsx</t>
+  </si>
+  <si>
+    <t>Number of violent crimes per 1,000 population</t>
+  </si>
+  <si>
+    <t>Child Neglect/Abuse</t>
+  </si>
+  <si>
+    <t>Not at Place level</t>
+  </si>
+  <si>
+    <t>HCI_AbuseNeglectChildren_741_CT_PL_CO_RE_CA-24-4-15.xlsx</t>
+  </si>
+  <si>
+    <t>violent_crime</t>
+  </si>
+  <si>
+    <t>child_abuse</t>
+  </si>
+  <si>
+    <t>Percent of children (under 18) reported with neglect or physical or sexual abuse (or maltreatment in general)</t>
+  </si>
+  <si>
+    <t>voted</t>
+  </si>
+  <si>
+    <t>HCI_RegisteredVoters_653_CA_CO_RE_PL_CT_5-1-14.xlsx</t>
+  </si>
+  <si>
+    <t>Voter Participation</t>
+  </si>
+  <si>
+    <t>2002;2004;2006;2008</t>
+  </si>
+  <si>
+    <t>The number of prople who voted as a percent of total number of registered voters</t>
+  </si>
+  <si>
+    <t>bad_water</t>
+  </si>
+  <si>
+    <t>2008-2012</t>
+  </si>
+  <si>
+    <t>Unsafe Drinking Water</t>
+  </si>
+  <si>
+    <t>HCI_DrinkingWater_CA_RE_CO_CD_PL_CT-A-N-6-19-14.xlsx; HCI_DrinkingWater_CA_RE_CO_CD_PL_CT-O-Y-6-19-14.xlsx</t>
+  </si>
+  <si>
+    <t>Number of people served by a community water system with at least one MLC/TT violation in the period 2008-2012 as a percent of total number of people served by community water systems</t>
+  </si>
+  <si>
+    <t>p_trans_acc</t>
+  </si>
+  <si>
+    <t>2008 (Sacremento County); 2012 (Bay Area, Southern Ca, San Diego County)</t>
+  </si>
+  <si>
+    <t>Access to Public Transit</t>
+  </si>
+  <si>
+    <t>RailFerryBus10_SCAG_Output9-5-13.xls; RailFerryBus10_SANDAG_Output8-29-13.xls; RailFerryBus10_MTC_Output_11-15-13.xls; RailFerryBus10_SACOG_Output-11-26-13.xls</t>
+  </si>
+  <si>
+    <t>Proportion of the population that resides within a ½ mile of a transit stop with a headway of 15 minutes or less during peak commute hours</t>
+  </si>
+  <si>
+    <t>traf_fatal</t>
+  </si>
+  <si>
+    <t>traf_sev</t>
+  </si>
+  <si>
+    <t>Road Traffic Injuries</t>
+  </si>
+  <si>
+    <t>HCI_RoadTrafficInjuries_753_CT_PL_CO_RE_R4_CA-12-17-13_A-N.xlsx; HCI_RoadTrafficInjuries_753_CT_PL_CO_12-17-13_O-Y.xlsx</t>
+  </si>
+  <si>
+    <t>2002;2003;2004;2005;2006;2007;2008;2009;2010;2002-2004;2005-2007;2008-2010</t>
+  </si>
+  <si>
+    <t>Rate of injuries over total population (injuries per 100,000 people) - Fatal</t>
+  </si>
+  <si>
+    <t>Rate of injuries over total population (injuries per 100,000 people) - Severe Injury</t>
+  </si>
+  <si>
+    <t>alc_off</t>
+  </si>
+  <si>
+    <t>alc_on</t>
+  </si>
+  <si>
+    <t>alc_tot</t>
+  </si>
+  <si>
+    <t>Proximity to Alcohol</t>
+  </si>
+  <si>
+    <t>HCI_AlcoholOutletsQ_774_CA_RE_CO_CD_PL_CT-A-N-5-16-14.xlsx; HCI_AlcoholOutletsQ_774_CO_CD_PL_CT-O-Y-5-16-14.xlsx</t>
+  </si>
+  <si>
+    <t>Percent of Population within 1/4 Mile of Alcohol Outlets - Off Site Consumption License</t>
+  </si>
+  <si>
+    <t>Percent of Population within 1/4 Mile of Alcohol Outlets - On Site Consumption License</t>
+  </si>
+  <si>
+    <t>Percent of Population within 1/4 Mile of Alcohol Outlets - All Licenses</t>
+  </si>
+  <si>
+    <t>Children Scoring 6 of 6 on FITNESSGRAM</t>
+  </si>
+  <si>
+    <t>hh_f</t>
+  </si>
+  <si>
+    <t>hh_f_child</t>
+  </si>
+  <si>
+    <t>hh_m</t>
+  </si>
+  <si>
+    <t>hh_m_child</t>
+  </si>
+  <si>
+    <t>hh_married</t>
+  </si>
+  <si>
+    <t>hh_married_child</t>
+  </si>
+  <si>
+    <t>hh_nonfam</t>
+  </si>
+  <si>
+    <t>hh_nonfam_solo</t>
+  </si>
+  <si>
+    <t>Household Type</t>
+  </si>
+  <si>
+    <t>2005-2007;2008-2010;2011-2013</t>
+  </si>
+  <si>
+    <t>HCI_HouseholdType_746_CARECOCDPLCT_Alameda-Monterey_24APR15.xlsx</t>
+  </si>
+  <si>
+    <t>Percent of households - Female householder, no husband present</t>
+  </si>
+  <si>
+    <t>Percent of households - Female householder, no husband present, with own children under 18 years</t>
+  </si>
+  <si>
+    <t>Percent of households - Male householder, no wife present</t>
+  </si>
+  <si>
+    <t>Percent of households - Male householder, no wife present, with own children under 18 years</t>
+  </si>
+  <si>
+    <t>Percent of households - Married couple</t>
+  </si>
+  <si>
+    <t>Percent of households - Married couple with own children under 18 years</t>
+  </si>
+  <si>
+    <t>Percent of households - Nonfamily households</t>
+  </si>
+  <si>
+    <t>Percent of households - Nonfamily households with householder living alone</t>
   </si>
 </sst>
 </file>
@@ -722,25 +917,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="150.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -748,10 +943,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>24</v>
@@ -766,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -774,10 +969,10 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -792,7 +987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -800,10 +995,10 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -818,7 +1013,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -826,10 +1021,10 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -844,7 +1039,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -852,10 +1047,10 @@
         <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="E5">
         <v>2009</v>
@@ -870,50 +1065,50 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -921,10 +1116,10 @@
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>63</v>
@@ -939,7 +1134,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -947,10 +1142,10 @@
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
         <v>63</v>
@@ -965,7 +1160,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -973,10 +1168,10 @@
         <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E11">
         <v>2011</v>
@@ -991,7 +1186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -999,10 +1194,10 @@
         <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
         <v>72</v>
@@ -1017,10 +1212,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1028,10 +1223,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="E14">
         <v>2010</v>
@@ -1046,7 +1241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1054,10 +1249,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="E15">
         <v>2010</v>
@@ -1072,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1080,10 +1275,10 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -1098,7 +1293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1106,10 +1301,10 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1124,7 +1319,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1132,10 +1327,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
@@ -1150,7 +1345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1158,10 +1353,10 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -1176,7 +1371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1184,10 +1379,10 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -1202,7 +1397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1210,10 +1405,10 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1228,7 +1423,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,10 +1431,10 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -1254,7 +1449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1262,10 +1457,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1280,7 +1475,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1288,10 +1483,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -1306,7 +1501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1314,10 +1509,10 @@
         <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
         <v>72</v>
@@ -1332,7 +1527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1340,16 +1535,16 @@
         <v>79</v>
       </c>
       <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
         <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>83</v>
       </c>
       <c r="G26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1357,10 +1552,10 @@
         <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -1375,7 +1570,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1383,10 +1578,10 @@
         <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E28">
         <v>2010</v>
@@ -1401,7 +1596,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1409,10 +1604,10 @@
         <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E29">
         <v>2010</v>
@@ -1427,7 +1622,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1435,10 +1630,10 @@
         <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -1453,7 +1648,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1461,10 +1656,10 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
@@ -1479,7 +1674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1487,10 +1682,10 @@
         <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
@@ -1505,7 +1700,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1513,10 +1708,10 @@
         <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
@@ -1529,6 +1724,540 @@
       </c>
       <c r="H33" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34">
+        <v>2015</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35">
+        <v>2015</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36">
+        <v>2010</v>
+      </c>
+      <c r="F36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37">
+        <v>2013</v>
+      </c>
+      <c r="F37" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38">
+        <v>2010</v>
+      </c>
+      <c r="F38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" t="s">
+        <v>140</v>
+      </c>
+      <c r="H41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>144</v>
+      </c>
+      <c r="G42" t="s">
+        <v>141</v>
+      </c>
+      <c r="H42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43">
+        <v>2014</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>147</v>
+      </c>
+      <c r="H43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44">
+        <v>2014</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>148</v>
+      </c>
+      <c r="H44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45">
+        <v>2014</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" t="s">
+        <v>156</v>
+      </c>
+      <c r="H47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" t="s">
+        <v>157</v>
+      </c>
+      <c r="H48" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" t="s">
+        <v>158</v>
+      </c>
+      <c r="H49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" t="s">
+        <v>82</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" t="s">
+        <v>159</v>
+      </c>
+      <c r="H50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" t="s">
+        <v>160</v>
+      </c>
+      <c r="H51" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>165</v>
+      </c>
+      <c r="G52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H52" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>165</v>
+      </c>
+      <c r="G53" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>165</v>
+      </c>
+      <c r="G54" t="s">
+        <v>163</v>
+      </c>
+      <c r="H54" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1560,8 +2289,28 @@
     <hyperlink ref="A31" r:id="rId25"/>
     <hyperlink ref="A32" r:id="rId26"/>
     <hyperlink ref="A33" r:id="rId27"/>
+    <hyperlink ref="A34" r:id="rId28"/>
+    <hyperlink ref="A35" r:id="rId29"/>
+    <hyperlink ref="A36" r:id="rId30"/>
+    <hyperlink ref="A37" r:id="rId31"/>
+    <hyperlink ref="A38" r:id="rId32"/>
+    <hyperlink ref="A39" r:id="rId33"/>
+    <hyperlink ref="A40" r:id="rId34"/>
+    <hyperlink ref="A41" r:id="rId35"/>
+    <hyperlink ref="A42" r:id="rId36"/>
+    <hyperlink ref="A43" r:id="rId37"/>
+    <hyperlink ref="A44" r:id="rId38"/>
+    <hyperlink ref="A45" r:id="rId39"/>
+    <hyperlink ref="A46:A47" r:id="rId40" display="http://www.cdph.ca.gov/programs/Pages/HealthyCommunityIndicators.aspx"/>
+    <hyperlink ref="A48" r:id="rId41"/>
+    <hyperlink ref="A49" r:id="rId42"/>
+    <hyperlink ref="A50" r:id="rId43"/>
+    <hyperlink ref="A51" r:id="rId44"/>
+    <hyperlink ref="A52" r:id="rId45"/>
+    <hyperlink ref="A53" r:id="rId46"/>
+    <hyperlink ref="A54" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2016.08.15 - Create maps and start presentation
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data_science\CA_Housing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crsalviati/Desktop/data_science/CA_Housing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -251,9 +254,6 @@
     <t>ozone</t>
   </si>
   <si>
-    <t>Mean number of unhrealthy days of ozone exposure</t>
-  </si>
-  <si>
     <t>PM25_zcta_place_co_region_ca4-14-13.xls</t>
   </si>
   <si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>Percent of households - Nonfamily households with householder living alone</t>
+  </si>
+  <si>
+    <t>Mean number of unhealthy days of ozone exposure</t>
   </si>
 </sst>
 </file>
@@ -919,23 +922,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="150.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -946,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>24</v>
@@ -961,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -972,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -987,7 +990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -1013,7 +1016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -1039,7 +1042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5">
         <v>2009</v>
@@ -1065,7 +1068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>52</v>
@@ -1074,13 +1077,13 @@
         <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -1088,13 +1091,13 @@
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>57</v>
       </c>
@@ -1102,13 +1105,13 @@
         <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
         <v>63</v>
@@ -1134,7 +1137,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>63</v>
@@ -1160,7 +1163,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11">
         <v>2011</v>
@@ -1186,7 +1189,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
         <v>72</v>
@@ -1209,13 +1212,13 @@
         <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14">
         <v>2010</v>
@@ -1241,7 +1244,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15">
         <v>2010</v>
@@ -1267,7 +1270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -1293,7 +1296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1319,7 +1322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
@@ -1345,7 +1348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -1371,7 +1374,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -1397,7 +1400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1423,7 +1426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -1449,7 +1452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1475,7 +1478,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -1501,18 +1504,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
         <v>72</v>
@@ -1521,41 +1524,41 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" t="s">
         <v>77</v>
       </c>
-      <c r="H25" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -1564,24 +1567,24 @@
         <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
         <v>90</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28">
         <v>2010</v>
@@ -1590,24 +1593,24 @@
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
         <v>90</v>
       </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29">
         <v>2010</v>
@@ -1616,24 +1619,24 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
         <v>97</v>
       </c>
-      <c r="C30" t="s">
-        <v>98</v>
-      </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -1642,102 +1645,102 @@
         <v>25</v>
       </c>
       <c r="G30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" t="s">
         <v>94</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
         <v>97</v>
       </c>
-      <c r="C31" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
         <v>102</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>95</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" t="s">
         <v>103</v>
       </c>
-      <c r="G32" t="s">
-        <v>96</v>
-      </c>
-      <c r="H32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="H33" t="s">
         <v>107</v>
       </c>
-      <c r="C33" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" t="s">
-        <v>104</v>
-      </c>
-      <c r="H33" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>109</v>
       </c>
-      <c r="C34" t="s">
-        <v>110</v>
-      </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34">
         <v>2015</v>
@@ -1746,24 +1749,24 @@
         <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" t="s">
         <v>109</v>
       </c>
-      <c r="C35" t="s">
-        <v>110</v>
-      </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35">
         <v>2015</v>
@@ -1772,206 +1775,206 @@
         <v>7</v>
       </c>
       <c r="G35" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" t="s">
         <v>112</v>
       </c>
-      <c r="H35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36">
         <v>2010</v>
       </c>
       <c r="F36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" t="s">
-        <v>119</v>
-      </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37">
         <v>2013</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G37" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" t="s">
         <v>123</v>
       </c>
-      <c r="H37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="C38" t="s">
-        <v>127</v>
-      </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38">
         <v>2010</v>
       </c>
       <c r="F38" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" t="s">
+        <v>124</v>
+      </c>
+      <c r="H38" t="s">
         <v>128</v>
       </c>
-      <c r="G38" t="s">
-        <v>125</v>
-      </c>
-      <c r="H38" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H39" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
         <v>143</v>
       </c>
-      <c r="C41" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" t="s">
-        <v>144</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>140</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" t="s">
-        <v>143</v>
-      </c>
-      <c r="C42" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" t="s">
-        <v>144</v>
-      </c>
-      <c r="G42" t="s">
-        <v>141</v>
-      </c>
-      <c r="H42" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43">
         <v>2014</v>
@@ -1980,24 +1983,24 @@
         <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H43" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44">
         <v>2014</v>
@@ -2006,24 +2009,24 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H44" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45">
         <v>2014</v>
@@ -2032,232 +2035,232 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" t="s">
-        <v>155</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="s">
+        <v>164</v>
+      </c>
+      <c r="G47" t="s">
+        <v>155</v>
+      </c>
+      <c r="H47" t="s">
         <v>166</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" t="s">
         <v>164</v>
       </c>
-      <c r="D47" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G48" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
         <v>165</v>
       </c>
-      <c r="G47" t="s">
-        <v>156</v>
-      </c>
-      <c r="H47" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>166</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" t="s">
         <v>164</v>
       </c>
-      <c r="D48" t="s">
-        <v>82</v>
-      </c>
-      <c r="E48" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="G49" t="s">
+        <v>157</v>
+      </c>
+      <c r="H49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
         <v>165</v>
       </c>
-      <c r="G48" t="s">
-        <v>157</v>
-      </c>
-      <c r="H48" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>166</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" t="s">
         <v>164</v>
       </c>
-      <c r="D49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="G50" t="s">
+        <v>158</v>
+      </c>
+      <c r="H50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
         <v>165</v>
       </c>
-      <c r="G49" t="s">
-        <v>158</v>
-      </c>
-      <c r="H49" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>166</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" t="s">
         <v>164</v>
       </c>
-      <c r="D50" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="G51" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
         <v>165</v>
       </c>
-      <c r="G50" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>166</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" t="s">
         <v>164</v>
       </c>
-      <c r="D51" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="G52" t="s">
+        <v>160</v>
+      </c>
+      <c r="H52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
         <v>165</v>
       </c>
-      <c r="G51" t="s">
-        <v>160</v>
-      </c>
-      <c r="H51" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
         <v>164</v>
       </c>
-      <c r="D52" t="s">
-        <v>82</v>
-      </c>
-      <c r="E52" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="G53" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
         <v>165</v>
       </c>
-      <c r="G52" t="s">
-        <v>161</v>
-      </c>
-      <c r="H52" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
         <v>164</v>
       </c>
-      <c r="D53" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" t="s">
-        <v>165</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>162</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>166</v>
-      </c>
-      <c r="C54" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" t="s">
-        <v>165</v>
-      </c>
-      <c r="G54" t="s">
-        <v>163</v>
-      </c>
-      <c r="H54" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2016.08.16 - Presentation work
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="209">
   <si>
     <t>Source File</t>
   </si>
@@ -555,13 +558,115 @@
   </si>
   <si>
     <t>Mean number of unhealthy days of ozone exposure</t>
+  </si>
+  <si>
+    <t>nocar</t>
+  </si>
+  <si>
+    <t>hh_fam</t>
+  </si>
+  <si>
+    <t>zri_sqft</t>
+  </si>
+  <si>
+    <t>hval_sqft</t>
+  </si>
+  <si>
+    <t>Percent of households inhabited by families.</t>
+  </si>
+  <si>
+    <t>Percent of residents whose mode of transport to work was walking, bicycle, or public transportation.</t>
+  </si>
+  <si>
+    <t>Total population, 2010.</t>
+  </si>
+  <si>
+    <t>Percent of population within 1/2 mile of parks, beach, open space, or coastline.</t>
+  </si>
+  <si>
+    <t>Gini index (measure of income inequality).</t>
+  </si>
+  <si>
+    <t>Median household income.</t>
+  </si>
+  <si>
+    <t>Average family size.</t>
+  </si>
+  <si>
+    <t>Jobs to housing ratio.</t>
+  </si>
+  <si>
+    <t>Jobs to employed residents ratio.</t>
+  </si>
+  <si>
+    <t>Mean number of unhealthy days of ozone exposure.</t>
+  </si>
+  <si>
+    <t>Mean ambient PM2.5 concentration.</t>
+  </si>
+  <si>
+    <t>Percent of population aged 25 years old and over attaining at least a high school degree or GED.</t>
+  </si>
+  <si>
+    <t>Percent of families living below the living wage.</t>
+  </si>
+  <si>
+    <t>livewage</t>
+  </si>
+  <si>
+    <t>poverty</t>
+  </si>
+  <si>
+    <t>Overall poverty rate (percent).</t>
+  </si>
+  <si>
+    <t>Unemployment rate (percent).</t>
+  </si>
+  <si>
+    <t>The number of prople who voted as a percent of total number of registered voters.</t>
+  </si>
+  <si>
+    <t>Number of people served by a community water system with at least one MLC/TT violation.</t>
+  </si>
+  <si>
+    <t>Number of severe traffic injuries per 100,000 people.</t>
+  </si>
+  <si>
+    <t>Percent of population within 1/4 mile of "on-site" consumption alcohol outlets.</t>
+  </si>
+  <si>
+    <t>Zillow Rental Index - median of the estimated monthly rent price of all homes, per square foot.</t>
+  </si>
+  <si>
+    <t>Median home vale per square foot ($).</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Zillow</t>
+  </si>
+  <si>
+    <t>HCI</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>P-Value</t>
+  </si>
+  <si>
+    <t>Rental Index (Sqft.)</t>
+  </si>
+  <si>
+    <t>Home Value (Sqft.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,19 +705,255 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Futura Medium"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Futura Medium"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Futura Medium"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Futura Medium"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -628,7 +969,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1"/>
@@ -636,6 +977,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -644,7 +1033,128 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF002060"/>
+          <bgColor theme="0" tint="-0.14993743705557422"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF002060"/>
+          <bgColor theme="0" tint="-0.14993743705557422"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -922,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2316,4 +2826,692 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId48"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="150.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="15"/>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="15"/>
+      <c r="C6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="15"/>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="15"/>
+      <c r="C8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="15"/>
+      <c r="C9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="15"/>
+      <c r="C10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="15"/>
+      <c r="C11" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="15"/>
+      <c r="C13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="15"/>
+      <c r="C14" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="15"/>
+      <c r="C15" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
+      <c r="C16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="15"/>
+      <c r="C17" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="15"/>
+      <c r="C18" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="15"/>
+      <c r="C19" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="15"/>
+      <c r="C20" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="15"/>
+      <c r="C21" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="14"/>
+      <c r="C22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B22"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:D3 C5:D22">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="30"/>
+      <c r="B1" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2016.08.17 - Maps and presentation work
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Dictionary - Formatted" sheetId="3" r:id="rId3"/>
-    <sheet name="LinReg Results" sheetId="4" r:id="rId4"/>
-    <sheet name="Lasso Results" sheetId="5" r:id="rId5"/>
+    <sheet name="Dictionary - Raw" sheetId="1" r:id="rId1"/>
+    <sheet name="Dictionary - Formatted" sheetId="3" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="205">
   <si>
     <t>Source File</t>
   </si>
@@ -646,43 +646,13 @@
   </si>
   <si>
     <t>HCI</t>
-  </si>
-  <si>
-    <t>Coefficient</t>
-  </si>
-  <si>
-    <t>P-Value</t>
-  </si>
-  <si>
-    <t>Rental Index (Sqft.)</t>
-  </si>
-  <si>
-    <t>Home Value (Sqft.)</t>
-  </si>
-  <si>
-    <t>Lasso Coefficient</t>
-  </si>
-  <si>
-    <t>Home Value</t>
-  </si>
-  <si>
-    <t>Rental Index</t>
-  </si>
-  <si>
-    <t>drop hh_fam: strong negative correlation with gini_index and nocar</t>
-  </si>
-  <si>
-    <t>drop unemp_rate: very strong negative correlation with median_hh_income</t>
-  </si>
-  <si>
-    <t>drop alc_on: strong positive correlation with nocar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,43 +711,6 @@
       <color theme="0"/>
       <name val="Futura Medium"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -799,7 +732,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -975,61 +908,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1041,7 +919,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1"/>
@@ -1061,17 +939,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1084,39 +957,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1125,91 +965,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1242,6 +998,183 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Chart1"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="M2" t="str">
+            <v>Frequency</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="L3">
+            <v>5</v>
+          </cell>
+          <cell r="M3">
+            <v>0</v>
+          </cell>
+          <cell r="N3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="L4">
+            <v>15</v>
+          </cell>
+          <cell r="M4">
+            <v>3</v>
+          </cell>
+          <cell r="N4">
+            <v>125</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>25</v>
+          </cell>
+          <cell r="M5">
+            <v>51</v>
+          </cell>
+          <cell r="N5">
+            <v>250</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>35</v>
+          </cell>
+          <cell r="M6">
+            <v>264</v>
+          </cell>
+          <cell r="N6">
+            <v>325</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="L7">
+            <v>45</v>
+          </cell>
+          <cell r="M7">
+            <v>681</v>
+          </cell>
+          <cell r="N7">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="L8">
+            <v>55</v>
+          </cell>
+          <cell r="M8">
+            <v>681</v>
+          </cell>
+          <cell r="N8">
+            <v>250</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="L9">
+            <v>65</v>
+          </cell>
+          <cell r="M9">
+            <v>264</v>
+          </cell>
+          <cell r="N9">
+            <v>200</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="L10">
+            <v>75</v>
+          </cell>
+          <cell r="M10">
+            <v>51</v>
+          </cell>
+          <cell r="N10">
+            <v>150</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="L11">
+            <v>85</v>
+          </cell>
+          <cell r="M11">
+            <v>3</v>
+          </cell>
+          <cell r="N11">
+            <v>110</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="L12">
+            <v>95</v>
+          </cell>
+          <cell r="M12">
+            <v>0</v>
+          </cell>
+          <cell r="N12">
+            <v>85</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="L13">
+            <v>105</v>
+          </cell>
+          <cell r="M13">
+            <v>0</v>
+          </cell>
+          <cell r="N13">
+            <v>65</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="L14">
+            <v>115</v>
+          </cell>
+          <cell r="M14">
+            <v>0</v>
+          </cell>
+          <cell r="N14">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="L15">
+            <v>125</v>
+          </cell>
+          <cell r="M15">
+            <v>0</v>
+          </cell>
+          <cell r="N15">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="L16">
+            <v>135</v>
+          </cell>
+          <cell r="M16">
+            <v>0</v>
+          </cell>
+          <cell r="N16">
+            <v>35</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1510,7 +1443,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2907,414 +2840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="150.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>140</v>
-      </c>
-      <c r="B37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>148</v>
-      </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>155</v>
-      </c>
-      <c r="B41" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>156</v>
-      </c>
-      <c r="B42" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>157</v>
-      </c>
-      <c r="B43" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>158</v>
-      </c>
-      <c r="B44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>161</v>
-      </c>
-      <c r="B47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>162</v>
-      </c>
-      <c r="B48" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3325,18 +2854,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>203</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -3347,7 +2876,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B3" s="23"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="15" t="s">
         <v>178</v>
       </c>
@@ -3356,7 +2885,7 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>204</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -3367,7 +2896,7 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="24"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
@@ -3376,7 +2905,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="24"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
@@ -3385,7 +2914,7 @@
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="24"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
@@ -3394,7 +2923,7 @@
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="24"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="9" t="s">
         <v>43</v>
       </c>
@@ -3403,7 +2932,7 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="24"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="10" t="s">
         <v>62</v>
       </c>
@@ -3412,7 +2941,7 @@
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="24"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
         <v>67</v>
       </c>
@@ -3421,7 +2950,7 @@
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="24"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="10" t="s">
         <v>73</v>
       </c>
@@ -3430,7 +2959,7 @@
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="24"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="9" t="s">
         <v>76</v>
       </c>
@@ -3439,7 +2968,7 @@
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="24"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="10" t="s">
         <v>86</v>
       </c>
@@ -3448,7 +2977,7 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="24"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
         <v>192</v>
       </c>
@@ -3457,7 +2986,7 @@
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="24"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="10" t="s">
         <v>193</v>
       </c>
@@ -3466,7 +2995,7 @@
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="24"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
         <v>103</v>
       </c>
@@ -3475,7 +3004,7 @@
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="24"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="10" t="s">
         <v>124</v>
       </c>
@@ -3484,7 +3013,7 @@
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="24"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
         <v>129</v>
       </c>
@@ -3494,7 +3023,7 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="24"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="10" t="s">
         <v>140</v>
       </c>
@@ -3503,7 +3032,7 @@
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="24"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="10" t="s">
         <v>147</v>
       </c>
@@ -3512,7 +3041,7 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="24"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="10" t="s">
         <v>175</v>
       </c>
@@ -3521,7 +3050,7 @@
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="25"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="11" t="s">
         <v>176</v>
       </c>
@@ -3535,326 +3064,10 @@
     <mergeCell ref="B4:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:D3 C5:D22">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="21"/>
-      <c r="B1" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="G3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="G4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="G5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="20"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="4" width="22.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="21">
-      <c r="B1" s="33"/>
-      <c r="C1" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="2:4" ht="21">
-      <c r="B2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="21">
-      <c r="B3" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="38">
-        <v>0</v>
-      </c>
-      <c r="D3" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="21">
-      <c r="B4" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="38">
-        <v>0</v>
-      </c>
-      <c r="D4" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="21">
-      <c r="B5" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="40">
-        <v>0.17</v>
-      </c>
-      <c r="D5" s="40">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="21">
-      <c r="B6" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="40">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D6" s="40">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="21">
-      <c r="B7" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="38">
-        <v>0</v>
-      </c>
-      <c r="D7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="21">
-      <c r="B8" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="38">
-        <v>0</v>
-      </c>
-      <c r="D8" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="21">
-      <c r="B9" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="38">
-        <v>0</v>
-      </c>
-      <c r="D9" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="21">
-      <c r="B10" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="40">
-        <v>-0.08</v>
-      </c>
-      <c r="D10" s="40">
-        <v>-0.09</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="21">
-      <c r="B11" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="38">
-        <v>0</v>
-      </c>
-      <c r="D11" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="21">
-      <c r="B12" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="38">
-        <v>0</v>
-      </c>
-      <c r="D12" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="21">
-      <c r="B13" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="38">
-        <v>0</v>
-      </c>
-      <c r="D13" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="21">
-      <c r="B14" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="38">
-        <v>0</v>
-      </c>
-      <c r="D14" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="21">
-      <c r="B15" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="40">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="D15" s="40">
-        <v>-0.03</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="21">
-      <c r="B16" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="38">
-        <v>0</v>
-      </c>
-      <c r="D16" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="21">
-      <c r="B17" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="38">
-        <v>0</v>
-      </c>
-      <c r="D17" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="21">
-      <c r="B18" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="38">
-        <v>0</v>
-      </c>
-      <c r="D18" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="21">
-      <c r="B19" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" s="40">
-        <v>0.13</v>
-      </c>
-      <c r="D19" s="40">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="21">
-      <c r="B20" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="C20" s="40">
-        <v>0.11</v>
-      </c>
-      <c r="D20" s="40">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="21">
-      <c r="B21" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C21" s="40">
-        <v>-0.03</v>
-      </c>
-      <c r="D21" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="23.25">
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
2016.08.18 - Completed presentation.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data_science\CA_Housing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crsalviati/Desktop/data_science/CA_Housing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary - Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Dictionary - Formatted" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -652,7 +652,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,18 +697,23 @@
       <name val="Futura Medium"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
+      <sz val="15"/>
+      <color theme="0"/>
       <name val="Futura Medium"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="15"/>
       <color rgb="FF002060"/>
       <name val="Futura Medium"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="0"/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Futura Medium"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
       <name val="Futura Medium"/>
     </font>
   </fonts>
@@ -727,7 +732,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -928,23 +933,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -969,7 +974,8 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <fgColor auto="1"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <border>
@@ -998,183 +1004,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Chart1"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="M2" t="str">
-            <v>Frequency</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="L3">
-            <v>5</v>
-          </cell>
-          <cell r="M3">
-            <v>0</v>
-          </cell>
-          <cell r="N3">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="L4">
-            <v>15</v>
-          </cell>
-          <cell r="M4">
-            <v>3</v>
-          </cell>
-          <cell r="N4">
-            <v>125</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5">
-            <v>25</v>
-          </cell>
-          <cell r="M5">
-            <v>51</v>
-          </cell>
-          <cell r="N5">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
-            <v>35</v>
-          </cell>
-          <cell r="M6">
-            <v>264</v>
-          </cell>
-          <cell r="N6">
-            <v>325</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="L7">
-            <v>45</v>
-          </cell>
-          <cell r="M7">
-            <v>681</v>
-          </cell>
-          <cell r="N7">
-            <v>300</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="L8">
-            <v>55</v>
-          </cell>
-          <cell r="M8">
-            <v>681</v>
-          </cell>
-          <cell r="N8">
-            <v>250</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="L9">
-            <v>65</v>
-          </cell>
-          <cell r="M9">
-            <v>264</v>
-          </cell>
-          <cell r="N9">
-            <v>200</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="L10">
-            <v>75</v>
-          </cell>
-          <cell r="M10">
-            <v>51</v>
-          </cell>
-          <cell r="N10">
-            <v>150</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="L11">
-            <v>85</v>
-          </cell>
-          <cell r="M11">
-            <v>3</v>
-          </cell>
-          <cell r="N11">
-            <v>110</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="L12">
-            <v>95</v>
-          </cell>
-          <cell r="M12">
-            <v>0</v>
-          </cell>
-          <cell r="N12">
-            <v>85</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="L13">
-            <v>105</v>
-          </cell>
-          <cell r="M13">
-            <v>0</v>
-          </cell>
-          <cell r="N13">
-            <v>65</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="L14">
-            <v>115</v>
-          </cell>
-          <cell r="M14">
-            <v>0</v>
-          </cell>
-          <cell r="N14">
-            <v>50</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="L15">
-            <v>125</v>
-          </cell>
-          <cell r="M15">
-            <v>0</v>
-          </cell>
-          <cell r="N15">
-            <v>40</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="L16">
-            <v>135</v>
-          </cell>
-          <cell r="M16">
-            <v>0</v>
-          </cell>
-          <cell r="N16">
-            <v>35</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1446,19 +1275,19 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="150.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1510,7 +1339,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1536,7 +1365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1562,7 +1391,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +1417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>52</v>
@@ -1603,7 +1432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -1617,7 +1446,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>57</v>
       </c>
@@ -1631,7 +1460,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1657,7 +1486,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1683,7 +1512,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1735,10 +1564,10 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1764,7 +1593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1790,7 +1619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1816,7 +1645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1842,7 +1671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1868,7 +1697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1894,7 +1723,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1920,7 +1749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1946,7 +1775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1972,7 +1801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1998,7 +1827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +1853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +1879,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -2067,7 +1896,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -2093,7 +1922,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -2119,7 +1948,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -2145,7 +1974,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -2171,7 +2000,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -2197,7 +2026,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2052,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -2249,7 +2078,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -2275,7 +2104,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -2301,7 +2130,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2156,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -2353,7 +2182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -2379,7 +2208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -2405,7 +2234,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -2431,7 +2260,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -2457,7 +2286,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -2483,7 +2312,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -2509,7 +2338,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -2535,7 +2364,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -2561,7 +2390,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -2575,7 +2404,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -2601,7 +2430,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -2627,7 +2456,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -2653,7 +2482,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -2679,7 +2508,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>14</v>
       </c>
@@ -2705,7 +2534,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>14</v>
       </c>
@@ -2731,7 +2560,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2586,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
@@ -2843,218 +2672,218 @@
   <dimension ref="B1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="114.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:4" ht="22" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>203</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1">
+    <row r="3" spans="2:4" ht="23" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="20"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B4" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B5" s="21"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B7" s="21"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B8" s="21"/>
       <c r="C8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B9" s="21"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B10" s="21"/>
       <c r="C10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="14" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B11" s="21"/>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B12" s="21"/>
       <c r="C12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="14" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="14" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B15" s="21"/>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="14" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" ht="22" x14ac:dyDescent="0.3">
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B17" s="21"/>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B19" s="21"/>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B20" s="21"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="14" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B21" s="21"/>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" ht="22" x14ac:dyDescent="0.3">
       <c r="B22" s="22"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="13" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>